<commit_message>
add tests for excel requirements module
</commit_message>
<xml_diff>
--- a/tests/data/excel/requirements_valid.xlsx
+++ b/tests/data/excel/requirements_valid.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hutschen/Repositories/mv-tool-fapi/tests/import/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hutschen/repositories/mv-tool-api/tests/data/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C44DDC6-2343-3146-A552-08D41D90BC07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE7EEAEF-E406-B244-8D3E-72609FA68D22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17000" xr2:uid="{11C4B917-36A0-4648-BAF7-1EAB0A0DEE5B}"/>
+    <workbookView xWindow="380" yWindow="760" windowWidth="28040" windowHeight="17000" xr2:uid="{11C4B917-36A0-4648-BAF7-1EAB0A0DEE5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -37,27 +37,9 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
   <si>
-    <t>Reference</t>
-  </si>
-  <si>
-    <t>Summary</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
     <t>Target Object</t>
   </si>
   <si>
-    <t>Compliance Status</t>
-  </si>
-  <si>
-    <t>Compliance Comment</t>
-  </si>
-  <si>
-    <t>Completion</t>
-  </si>
-  <si>
     <t>R1</t>
   </si>
   <si>
@@ -143,6 +125,24 @@
   </si>
   <si>
     <t>Client</t>
+  </si>
+  <si>
+    <t>Requirement Reference</t>
+  </si>
+  <si>
+    <t>Requirement Summary</t>
+  </si>
+  <si>
+    <t>Requirement Description</t>
+  </si>
+  <si>
+    <t>Requirement Compliance Status</t>
+  </si>
+  <si>
+    <t>Requirement Compliance Comment</t>
+  </si>
+  <si>
+    <t>Requirement Completion Progress</t>
   </si>
 </sst>
 </file>
@@ -189,7 +189,7 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -208,20 +208,20 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{14812112-A76C-5C4F-B389-78B71C96923F}" name="Tabelle1" displayName="Tabelle1" ref="A1:G6" totalsRowShown="0">
   <autoFilter ref="A1:G6" xr:uid="{14812112-A76C-5C4F-B389-78B71C96923F}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{465D2CB5-B19B-6D43-864C-3FC510E382DF}" name="Reference"/>
-    <tableColumn id="2" xr3:uid="{9A8E9A0E-EAAC-0C4D-BE64-C4AADAC4FC54}" name="Summary"/>
-    <tableColumn id="3" xr3:uid="{D4A01C2D-68F7-9A45-90E6-C8CD441F35CC}" name="Description"/>
+    <tableColumn id="1" xr3:uid="{465D2CB5-B19B-6D43-864C-3FC510E382DF}" name="Requirement Reference"/>
+    <tableColumn id="2" xr3:uid="{9A8E9A0E-EAAC-0C4D-BE64-C4AADAC4FC54}" name="Requirement Summary"/>
+    <tableColumn id="3" xr3:uid="{D4A01C2D-68F7-9A45-90E6-C8CD441F35CC}" name="Requirement Description"/>
     <tableColumn id="4" xr3:uid="{9AEE37C6-18AE-8B45-9B97-4A937236EEFD}" name="Target Object"/>
-    <tableColumn id="5" xr3:uid="{29180FE0-B618-734E-BC43-811FD8C7A4F7}" name="Compliance Status"/>
-    <tableColumn id="6" xr3:uid="{CE8B9651-50A0-A441-98C4-7184CBCE7540}" name="Compliance Comment"/>
-    <tableColumn id="8" xr3:uid="{114E165A-8367-AB43-BE52-97A627D9F5B3}" name="Completion"/>
+    <tableColumn id="5" xr3:uid="{29180FE0-B618-734E-BC43-811FD8C7A4F7}" name="Requirement Compliance Status"/>
+    <tableColumn id="6" xr3:uid="{CE8B9651-50A0-A441-98C4-7184CBCE7540}" name="Requirement Compliance Comment"/>
+    <tableColumn id="8" xr3:uid="{114E165A-8367-AB43-BE52-97A627D9F5B3}" name="Requirement Completion Progress"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -520,7 +520,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -531,50 +531,51 @@
     <col min="4" max="4" width="14.6640625" customWidth="1"/>
     <col min="5" max="5" width="18.6640625" customWidth="1"/>
     <col min="6" max="6" width="21.5" customWidth="1"/>
+    <col min="7" max="7" width="32.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="G1" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="G2" s="1">
         <v>1</v>
@@ -582,22 +583,22 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E3" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="F3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="G3" s="1">
         <v>1</v>
@@ -605,22 +606,22 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E4" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="F4" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="G4" s="1">
         <v>1</v>
@@ -628,22 +629,22 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E5" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="F5" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="G5" s="1">
         <v>1</v>
@@ -651,22 +652,22 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D6" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="E6" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F6" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="G6" s="1">
         <v>1</v>

</xml_diff>